<commit_message>
page updated for advertisement
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="schedule" vbProcedure="false">Sheet1!$A$1:$K$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="schedule" vbProcedure="false">Sheet1!$A$1:$K$23</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -112,10 +112,10 @@
     <t xml:space="preserve">Lokesh Mano</t>
   </si>
   <si>
-    <t xml:space="preserve">Coffee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advanced and combining plots</t>
+    <t xml:space="preserve">Break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced ggplot</t>
   </si>
   <si>
     <t xml:space="preserve">Lunch</t>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t xml:space="preserve">Wrap-up day II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Break</t>
   </si>
   <si>
     <t xml:space="preserve">Restaurang Valvet</t>
@@ -301,37 +298,41 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -587,13 +588,13 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="30"/>
@@ -860,8 +861,8 @@
       <c r="J16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3" t="n">
         <v>0.5625</v>
       </c>
@@ -875,8 +876,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="3" t="n">
         <v>0.645833333333333</v>
       </c>
@@ -891,8 +892,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="3" t="n">
         <v>0.6875</v>
       </c>
@@ -908,141 +909,141 @@
       <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="C20" s="3" t="n">
-        <v>0.708333333333333</v>
+        <v>0.770833333333333</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>0.770833333333333</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0" t="s">
-        <v>34</v>
+      <c r="K20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>0.770833333333333</v>
+        <v>0.375</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>0.916666666666667</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="n">
-        <v>0.375</v>
+        <v>0.427083333333333</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>0.427083333333333</v>
-      </c>
-      <c r="E22" s="7" t="s">
+        <v>0.4375</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="3" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="3" t="n">
-        <v>0.427083333333333</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>18</v>
+      <c r="F23" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="3" t="n">
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E24" s="7" t="s">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="3" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>0.541666666666667</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="3" t="n">
-        <v>0.541666666666667</v>
+        <v>0.625</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>17</v>
+        <v>0.645833333333333</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="3" t="n">
-        <v>0.625</v>
+        <v>0.645833333333333</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>0.645833333333333</v>
+        <v>0.6875</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="n">
-        <v>0.645833333333333</v>
+        <v>0.6875</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>0.6875</v>
+        <v>0.697916666666667</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F28" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="3" t="n">
-        <v>0.6875</v>
+        <v>0.697916666666667</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>0.697916666666667</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>42</v>
@@ -1051,20 +1052,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="3" t="n">
-        <v>0.697916666666667</v>
-      </c>
-      <c r="D30" s="3" t="n">
-        <v>0.708333333333333</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
shiny slides 1 and 2
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -172,7 +172,13 @@
     <t xml:space="preserve">Intro to R-Shiny app</t>
   </si>
   <si>
+    <t xml:space="preserve">topics/Shiny/slide_shiny1.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">R-Shiny apps part-II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topics/Shiny/slide_shiny2.html</t>
   </si>
   <si>
     <t xml:space="preserve">R-Shiny apps part-III</t>
@@ -587,14 +593,14 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="30"/>
@@ -946,6 +952,9 @@
       <c r="F21" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="K21" s="5" t="s">
         <v>15</v>
       </c>
@@ -970,10 +979,13 @@
         <v>0.5</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J23" s="6"/>
     </row>
@@ -996,7 +1008,7 @@
         <v>0.625</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>17</v>
@@ -1021,7 +1033,7 @@
         <v>0.6875</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,7 +1044,7 @@
         <v>0.697916666666667</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>17</v>
@@ -1046,7 +1058,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
updated contents and schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -121,10 +121,16 @@
     <t xml:space="preserve">Advanced ggplot</t>
   </si>
   <si>
+    <t xml:space="preserve">topics/ggplot/slide_gg2.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lunch</t>
   </si>
   <si>
     <t xml:space="preserve">Vector and bitmap images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topics/others_day1/Vector_Bitmap_Images.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">PCA plots</t>
@@ -618,7 +624,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -736,6 +742,9 @@
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="n">
@@ -745,7 +754,7 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J6" s="6"/>
     </row>
@@ -757,10 +766,13 @@
         <v>0.5625</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,7 +783,7 @@
         <v>0.625</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>14</v>
@@ -785,7 +797,7 @@
         <v>0.645833333333333</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,7 +808,7 @@
         <v>0.6875</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>17</v>
@@ -810,7 +822,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>17</v>
@@ -818,7 +830,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -830,13 +842,13 @@
         <v>0.427083333333333</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="5" t="s">
@@ -863,13 +875,13 @@
         <v>0.5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,7 +892,7 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J15" s="6"/>
     </row>
@@ -892,13 +904,13 @@
         <v>0.625</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -912,7 +924,7 @@
         <v>0.645833333333333</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
@@ -927,7 +939,7 @@
         <v>0.6875</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>17</v>
@@ -943,7 +955,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>17</v>
@@ -953,7 +965,7 @@
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
       <c r="B20" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>0.770833333333333</v>
@@ -962,16 +974,16 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
@@ -983,16 +995,16 @@
         <v>0.427083333333333</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>15</v>
@@ -1018,16 +1030,16 @@
         <v>0.5</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J23" s="6"/>
     </row>
@@ -1039,7 +1051,7 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,16 +1062,16 @@
         <v>0.625</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,7 +1082,7 @@
         <v>0.645833333333333</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1093,7 @@
         <v>0.6875</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,7 +1104,7 @@
         <v>0.697916666666667</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>17</v>
@@ -1106,7 +1118,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
gg labs and download page
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -115,6 +115,9 @@
     <t xml:space="preserve">topics/ggplot/slide_gg1.html</t>
   </si>
   <si>
+    <t xml:space="preserve">topics/ggplot/lab_gg1.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Break</t>
   </si>
   <si>
@@ -122,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">topics/ggplot/slide_gg2.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topics/ggplot/lab_gg2.html</t>
   </si>
   <si>
     <t xml:space="preserve">Lunch</t>
@@ -334,7 +340,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,6 +363,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -624,7 +634,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -700,7 +710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="3" t="n">
         <v>0.385416666666667</v>
       </c>
@@ -716,7 +726,10 @@
       <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="3" t="n">
@@ -726,10 +739,10 @@
         <v>0.4375</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="3" t="n">
         <v>0.4375</v>
       </c>
@@ -737,13 +750,16 @@
         <v>0.5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,9 +770,9 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="n">
@@ -765,14 +781,14 @@
       <c r="D7" s="3" t="n">
         <v>0.5625</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>23</v>
+      <c r="E7" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +799,7 @@
         <v>0.625</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>14</v>
@@ -797,7 +813,7 @@
         <v>0.645833333333333</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,7 +824,7 @@
         <v>0.6875</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>17</v>
@@ -822,7 +838,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>17</v>
@@ -830,7 +846,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -842,15 +858,15 @@
         <v>0.427083333333333</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="J12" s="7"/>
       <c r="K12" s="5" t="s">
         <v>15</v>
       </c>
@@ -863,9 +879,9 @@
         <v>0.4375</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="3" t="n">
@@ -875,13 +891,13 @@
         <v>0.5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,9 +908,9 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="3" t="n">
@@ -904,19 +920,19 @@
         <v>0.625</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="3" t="n">
         <v>0.5625</v>
       </c>
@@ -924,14 +940,14 @@
         <v>0.645833333333333</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="J17" s="7"/>
       <c r="K17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="3" t="n">
         <v>0.645833333333333</v>
       </c>
@@ -939,15 +955,15 @@
         <v>0.6875</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="3" t="n">
         <v>0.6875</v>
       </c>
@@ -955,17 +971,17 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="6"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8" t="s">
-        <v>39</v>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>0.770833333333333</v>
@@ -974,16 +990,16 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="J20" s="7"/>
       <c r="K20" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
@@ -994,17 +1010,17 @@
       <c r="D21" s="3" t="n">
         <v>0.427083333333333</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>43</v>
+      <c r="E21" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>15</v>
@@ -1018,9 +1034,9 @@
         <v>0.4375</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="J22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="3" t="n">
@@ -1029,19 +1045,19 @@
       <c r="D23" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>46</v>
+      <c r="E23" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J23" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="J23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="3" t="n">
@@ -1051,7 +1067,7 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,17 +1077,17 @@
       <c r="D25" s="3" t="n">
         <v>0.625</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>49</v>
+      <c r="E25" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,7 +1098,7 @@
         <v>0.645833333333333</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,7 +1109,7 @@
         <v>0.6875</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,7 +1120,7 @@
         <v>0.697916666666667</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>17</v>
@@ -1118,7 +1134,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
changed event order and names
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="schedule" vbProcedure="false">Sheet1!$A$1:$K$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="schedule" vbProcedure="false">Sheet1!$A$1:$K$25</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Lunch</t>
   </si>
   <si>
-    <t xml:space="preserve">Vector and bitmap images</t>
+    <t xml:space="preserve">Vector and bitmap</t>
   </si>
   <si>
     <t xml:space="preserve">topics/others_day1/Vector_Bitmap_Images.pdf</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Fika</t>
   </si>
   <si>
-    <t xml:space="preserve">Single-cell data visualizations</t>
+    <t xml:space="preserve">Single-cell</t>
   </si>
   <si>
     <t xml:space="preserve">Wrap-up day I</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">14/05/2025</t>
   </si>
   <si>
-    <t xml:space="preserve">Intro to Quarto</t>
+    <t xml:space="preserve">Quarto</t>
   </si>
   <si>
     <t xml:space="preserve">Katja Kozjek</t>
@@ -178,19 +178,25 @@
     <t xml:space="preserve">topics/Quarto/lab_quarto1.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Advanced Quarto</t>
+    <t xml:space="preserve">Quarto (continuation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic plotting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topics/dynamic_plotting/slide_dynamic_plot1.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic plotting (continuation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarto Dashboards</t>
   </si>
   <si>
     <t xml:space="preserve">topics/Quarto/slide_quarto2.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Intro to dynamic plotting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">topics/dynamic_plotting/slide_dynamic_plot1.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advanced dynamic plotting</t>
+    <t xml:space="preserve">Quarto Dashboards (continuation)</t>
   </si>
   <si>
     <t xml:space="preserve">Wrap-up day II</t>
@@ -644,8 +650,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -920,177 +926,176 @@
         <v>0.4375</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>0.5</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="D15" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="D15" s="3" t="n">
-        <v>0.541666666666667</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="3" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="E16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="3" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="3" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="D18" s="3" t="n">
         <v>0.625</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="3" t="n">
-        <v>0.5625</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>0.645833333333333</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="3" t="n">
-        <v>0.645833333333333</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>0.6875</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="3" t="n">
-        <v>0.6875</v>
+        <v>0.5625</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>0.708333333333333</v>
+        <v>0.645833333333333</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H19" s="8"/>
       <c r="J19" s="7"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="3" t="n">
+        <v>0.645833333333333</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="3" t="n">
-        <v>0.770833333333333</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>0.916666666666667</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="3" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="3" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>0.427083333333333</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="1" t="s">
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="3" t="n">
-        <v>0.427083333333333</v>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="3" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>17</v>
@@ -1099,33 +1104,36 @@
         <v>18</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J23" s="7"/>
+      <c r="K23" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="3" t="n">
-        <v>0.5</v>
+        <v>0.427083333333333</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>0.541666666666667</v>
+        <v>0.4375</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="3" t="n">
-        <v>0.541666666666667</v>
+        <v>0.4375</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>17</v>
@@ -1134,64 +1142,97 @@
         <v>18</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="J25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="3" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D27" s="3" t="n">
         <v>0.625</v>
       </c>
-      <c r="D26" s="3" t="n">
-        <v>0.645833333333333</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="3" t="n">
-        <v>0.645833333333333</v>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>0.6875</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="n">
-        <v>0.6875</v>
+        <v>0.625</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>0.697916666666667</v>
+        <v>0.645833333333333</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="3" t="n">
-        <v>0.697916666666667</v>
+        <v>0.645833333333333</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>0.708333333333333</v>
+        <v>0.6875</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="1" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="3" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>0.697916666666667</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="3" t="n">
+        <v>0.697916666666667</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
single-cell & dashboard start
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -157,6 +157,9 @@
     <t xml:space="preserve">Single-cell</t>
   </si>
   <si>
+    <t xml:space="preserve">topics/ggplot/lab_sc.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wrap-up day I</t>
   </si>
   <si>
@@ -194,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">topics/Quarto/slide_quarto2.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topics/Quarto/lab_quarto2.html</t>
   </si>
   <si>
     <t xml:space="preserve">Quarto Dashboards (continuation)</t>
@@ -650,8 +656,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -861,6 +867,9 @@
       <c r="G10" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I10" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="3" t="n">
@@ -870,7 +879,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>17</v>
@@ -878,7 +887,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -890,19 +899,19 @@
         <v>0.427083333333333</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="5" t="s">
@@ -929,13 +938,13 @@
         <v>0.458333333333333</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H14" s="8"/>
     </row>
@@ -947,16 +956,16 @@
         <v>0.5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,13 +988,13 @@
         <v>0.583333333333333</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J17" s="7"/>
     </row>
@@ -997,16 +1006,19 @@
         <v>0.625</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="J18" s="7"/>
     </row>
@@ -1036,13 +1048,13 @@
         <v>0.6875</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,7 +1067,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>17</v>
@@ -1065,7 +1077,7 @@
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>0.770833333333333</v>
@@ -1074,16 +1086,16 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
@@ -1095,7 +1107,7 @@
         <v>0.427083333333333</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>17</v>
@@ -1104,10 +1116,10 @@
         <v>18</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>15</v>
@@ -1133,7 +1145,7 @@
         <v>0.5</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>17</v>
@@ -1142,10 +1154,10 @@
         <v>18</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J25" s="7"/>
     </row>
@@ -1168,7 +1180,7 @@
         <v>0.625</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>17</v>
@@ -1177,10 +1189,10 @@
         <v>18</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,7 +1214,7 @@
         <v>0.6875</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,7 +1225,7 @@
         <v>0.697916666666667</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>17</v>
@@ -1227,7 +1239,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
sc until raw qc
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">topics/dynamic_plotting/slide_dynamic_plot1.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topics/dynamic_plotting/lab_dynamic_plot1.html</t>
   </si>
   <si>
     <t xml:space="preserve">Dynamic plotting (continuation)</t>
@@ -657,7 +660,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -668,8 +671,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="44.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="44.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="1" width="10.66"/>
@@ -967,6 +969,9 @@
       <c r="H15" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="I15" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="3" t="n">
@@ -988,7 +993,7 @@
         <v>0.583333333333333</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>37</v>
@@ -1006,7 +1011,7 @@
         <v>0.625</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>37</v>
@@ -1015,10 +1020,10 @@
         <v>38</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J18" s="7"/>
     </row>
@@ -1048,7 +1053,7 @@
         <v>0.6875</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>37</v>
@@ -1067,7 +1072,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>17</v>
@@ -1077,7 +1082,7 @@
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>0.770833333333333</v>
@@ -1086,16 +1091,16 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
@@ -1107,7 +1112,7 @@
         <v>0.427083333333333</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>17</v>
@@ -1116,10 +1121,10 @@
         <v>18</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>15</v>
@@ -1145,7 +1150,7 @@
         <v>0.5</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>17</v>
@@ -1154,10 +1159,10 @@
         <v>18</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J25" s="7"/>
     </row>
@@ -1180,7 +1185,7 @@
         <v>0.625</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>17</v>
@@ -1189,10 +1194,10 @@
         <v>18</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,7 +1219,7 @@
         <v>0.6875</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,7 +1230,7 @@
         <v>0.697916666666667</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>17</v>
@@ -1239,7 +1244,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
shortened topics in schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -184,7 +184,7 @@
     <t xml:space="preserve">Quarto (continuation)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dynamic plotting</t>
+    <t xml:space="preserve">Dynamic plots</t>
   </si>
   <si>
     <t xml:space="preserve">topics/dynamic_plotting/slide_dynamic_plot1.html</t>
@@ -193,10 +193,10 @@
     <t xml:space="preserve">topics/dynamic_plotting/lab_dynamic_plot1.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Dynamic plotting (continuation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quarto Dashboards</t>
+    <t xml:space="preserve">Dynamic plots (continuation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboards</t>
   </si>
   <si>
     <t xml:space="preserve">topics/Quarto/slide_quarto2.html</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">topics/Quarto/lab_quarto2.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Quarto Dashboards (continuation)</t>
+    <t xml:space="preserve">Dashboards (continuation)</t>
   </si>
   <si>
     <t xml:space="preserve">Wrap-up day II</t>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">15/05/2025</t>
   </si>
   <si>
-    <t xml:space="preserve">Intro to R-Shiny app</t>
+    <t xml:space="preserve">Intro to R-Shiny</t>
   </si>
   <si>
     <t xml:space="preserve">topics/Shiny/slide_shiny1.html</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">topics/Shiny/lab_shiny1.html</t>
   </si>
   <si>
-    <t xml:space="preserve">R-Shiny apps part-II</t>
+    <t xml:space="preserve">R-Shiny part-II</t>
   </si>
   <si>
     <t xml:space="preserve">topics/Shiny/slide_shiny2.html</t>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">topics/Shiny/lab_shiny2.html</t>
   </si>
   <si>
-    <t xml:space="preserve">R-Shiny apps part-III</t>
+    <t xml:space="preserve">R-Shiny part-III</t>
   </si>
   <si>
     <t xml:space="preserve">topics/Shiny/slide_shiny3.html</t>
@@ -660,7 +660,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>